<commit_message>
Update Strain background of all chemicals.xlsx
</commit_message>
<xml_diff>
--- a/result_ecYeast/Strain background of all chemicals.xlsx
+++ b/result_ecYeast/Strain background of all chemicals.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="560" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="343">
   <si>
     <t>Chemicals</t>
   </si>
@@ -1207,6 +1207,53 @@
   </si>
   <si>
     <t>glucose</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ecS-adenosyl-L-methionine.mat</t>
+  </si>
+  <si>
+    <t>ec2_Fucosyllactose.mat</t>
+  </si>
+  <si>
+    <t>ecLycopene.mat</t>
+  </si>
+  <si>
+    <t>S-adenosyl-L-methionine</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>2'-fucosyllactose</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>lycopene</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>xylose + lactose</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>glucose</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>YOL052C</t>
+  </si>
+  <si>
+    <t>YDR502C</t>
+  </si>
+  <si>
+    <t>YDL236W,YPL061W</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>YML075C,YMR303C,YPL061W,YPL188W,YMR165C,YNR016C,YGL055W</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>YBR020W,YBR018C,YBR019C,YLR300W</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -2146,7 +2193,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2154,15 +2201,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XES118"/>
+  <dimension ref="A1:XES121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="D121" sqref="D121"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
+      <selection activeCell="J121" sqref="J121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.75" customWidth="1"/>
+    <col min="1" max="1" width="23.125" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
     <col min="5" max="5" width="15.5" customWidth="1"/>
     <col min="6" max="6" width="11.875" customWidth="1"/>
@@ -20488,6 +20535,63 @@
         <v>329</v>
       </c>
     </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A119" t="s">
+        <v>333</v>
+      </c>
+      <c r="B119" t="s">
+        <v>330</v>
+      </c>
+      <c r="C119" t="s">
+        <v>2</v>
+      </c>
+      <c r="D119" t="s">
+        <v>329</v>
+      </c>
+      <c r="E119" t="s">
+        <v>339</v>
+      </c>
+      <c r="G119" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A120" t="s">
+        <v>334</v>
+      </c>
+      <c r="B120" t="s">
+        <v>331</v>
+      </c>
+      <c r="C120" t="s">
+        <v>2</v>
+      </c>
+      <c r="D120" t="s">
+        <v>336</v>
+      </c>
+      <c r="G120" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A121" t="s">
+        <v>335</v>
+      </c>
+      <c r="B121" t="s">
+        <v>332</v>
+      </c>
+      <c r="C121" t="s">
+        <v>2</v>
+      </c>
+      <c r="D121" t="s">
+        <v>337</v>
+      </c>
+      <c r="E121" t="s">
+        <v>341</v>
+      </c>
+      <c r="G121" t="s">
+        <v>342</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A1:G116">
     <sortCondition ref="B1:B116"/>

</xml_diff>